<commit_message>
pip freeze -> requirements.txt
</commit_message>
<xml_diff>
--- a/outpack.xlsx
+++ b/outpack.xlsx
@@ -455,10 +455,10 @@
   <dimension ref="A1:F129"/>
   <sheetViews>
     <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="1" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A8" activeCellId="0" sqref="A8"/>
+      <selection pane="topLeft" activeCell="A9" activeCellId="0" sqref="A9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="0" outlineLevelRow="0"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="11.53515625" defaultRowHeight="12.75" zeroHeight="0" outlineLevelRow="0"/>
   <cols>
     <col width="13" customWidth="1" style="1" min="1" max="1"/>
     <col width="50" customWidth="1" style="1" min="2" max="2"/>

</xml_diff>